<commit_message>
add graphic for a tipo de aprendizaje
</commit_message>
<xml_diff>
--- a/for_git/04-10-24.xlsx
+++ b/for_git/04-10-24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SECU-04\Documents\for_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AE4120-D303-4732-9D90-BEAB98587C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89BFB48-750D-4FD0-9C02-5F5C005A95B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4140" windowWidth="21600" windowHeight="11385" xr2:uid="{873D8AB2-7E1A-410D-8C42-4EC1C7F54FE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{873D8AB2-7E1A-410D-8C42-4EC1C7F54FE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,9 +138,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -161,6 +158,1747 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Gabriela</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$G$43:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B535-4ED0-9F0F-29BC0A7F9F9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Felipe</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$43:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E8E5-4F83-9E15-67A0859FA49B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56152991-50EC-8F20-D668-2A865E51F250}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADD7B035-B2B6-2716-2C61-0C55DCCFDEA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,7 +2201,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,16 +2210,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -507,7 +2245,7 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
@@ -1360,5 +3098,6 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>